<commit_message>
se agregó estructura de control de versión y se modificó documentos
</commit_message>
<xml_diff>
--- a/Entregables/IV. Métodos de comunicación del equipo de trabajo/IV.2 Plan de Comunicaciones/APPMO-SP_PCO_v1.0.xlsx
+++ b/Entregables/IV. Métodos de comunicación del equipo de trabajo/IV.2 Plan de Comunicaciones/APPMO-SP_PCO_v1.0.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
   <si>
     <t>PLAN DE COMUNICACIÓN</t>
   </si>
@@ -282,13 +282,49 @@
   </si>
   <si>
     <t>Usuarios del producto</t>
+  </si>
+  <si>
+    <t>CONTROL DE VERSIONES</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>Hecha por</t>
+  </si>
+  <si>
+    <t>Revisada por</t>
+  </si>
+  <si>
+    <t>Aprobada por</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>TDCJ</t>
+  </si>
+  <si>
+    <t>FJHH</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>SIGLAS DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>ADMINISTRACIÓN DE LA APLICACIÓN MÓVIL DE LA PANADERÍA SAN PEDRO</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -324,8 +360,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +392,20 @@
         <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -393,28 +447,45 @@
       <left style="hair">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,7 +510,40 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,507 +894,596 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L23"/>
+  <dimension ref="B3:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5546875"/>
     <col min="2" max="2" width="4.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="6" max="6" width="22.77734375" customWidth="1"/>
-    <col min="7" max="8" width="11.5546875"/>
+    <col min="7" max="7" width="11.5546875"/>
+    <col min="8" max="8" width="18.44140625" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" customWidth="1"/>
     <col min="10" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="2:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="17">
+        <v>43487</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="2:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="2:12" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="12" spans="2:12" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="13">
-        <v>43640</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G6" s="2" t="s">
+      <c r="L14" s="10">
+        <v>43489</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+    <row r="18" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J18" s="8">
         <v>43472</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L18" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+    <row r="19" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J19" s="8">
         <v>43472</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L19" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+    <row r="20" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J20" s="8">
         <v>43475</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L20" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+    <row r="21" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D21" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J21" s="8">
         <v>43477</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L21" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="66" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+    <row r="22" spans="2:12" ht="66" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>5</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C22" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H22" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J22" s="8">
         <v>43481</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L22" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+    <row r="23" spans="2:12" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
         <v>6</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D23" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H23" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J23" s="8">
         <v>43482</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L23" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+    <row r="24" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3">
         <v>7</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D24" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H24" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J24" s="8">
         <v>43494</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L24" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="66" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+    <row r="25" spans="2:12" ht="66" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
         <v>8</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G25" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J25" s="8">
         <v>43500</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K25" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L25" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+    <row r="26" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C26" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D26" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J26" s="8">
         <v>43642</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K26" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L26" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+    <row r="27" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
         <v>10</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C27" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E27" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H27" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J27" s="8">
         <v>43686</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K27" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L27" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+    <row r="28" spans="2:12" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
         <v>11</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D28" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E28" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G28" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J28" s="8">
         <v>43686</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K28" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="L18" s="10"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
+      <c r="L28" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:L6"/>
+  <mergeCells count="9">
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1321,135 +1514,135 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="5" spans="2:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>